<commit_message>
Fixed R8 in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25744</t>
   </si>
   <si>
     <t xml:space="preserve">R9</t>
@@ -418,29 +421,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1A1A1A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -511,11 +491,11 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.93"/>
@@ -861,7 +841,7 @@
         <v>52</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,16 +849,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,16 +866,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,16 +883,16 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,16 +900,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,16 +917,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,16 +934,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>